<commit_message>
Completed Results + Updated Methodology
Results were completed and updated alongside prompts added into the appropriate folders.

Methodology also updated to add prompt examples and Appendix
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Repo\Dissertation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7286EE-6FF4-4423-974B-6576FB1545AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C49FC1-7F9E-421C-B959-D3FFEA5FB0DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9480" yWindow="1365" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{6E62CC2F-5E46-4B0F-9F3F-D109107C993D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{6E62CC2F-5E46-4B0F-9F3F-D109107C993D}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1277" uniqueCount="98">
   <si>
     <t>Section</t>
   </si>
@@ -475,7 +475,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
@@ -503,17 +503,7 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -857,8 +847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E456A3C5-04F2-4269-B1CC-66B09066F0AA}">
   <dimension ref="A1:I86"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:I81"/>
+    <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83:E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2834,10 +2824,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F11B0BFB-3F43-4298-9582-F5223F20D3AC}">
-  <dimension ref="A1:I81"/>
+  <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:XFD41"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3465,27 +3455,27 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
+    <row r="27" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="C27" s="19">
+      <c r="B27" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" s="8">
         <v>2</v>
       </c>
-      <c r="D27" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="E27" s="20" t="str">
+      <c r="D27" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" s="15" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\2EIGRP\router22.png","Prompt26")</f>
         <v>Prompt26</v>
       </c>
-      <c r="F27" s="18" t="s">
+      <c r="F27" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="G27" s="18" t="s">
+      <c r="G27" s="3" t="s">
         <v>89</v>
       </c>
     </row>
@@ -3499,7 +3489,7 @@
       <c r="C28" s="10">
         <v>2</v>
       </c>
-      <c r="D28" s="21" t="s">
+      <c r="D28" s="5" t="s">
         <v>46</v>
       </c>
       <c r="E28" s="6" t="str">
@@ -3523,7 +3513,7 @@
       <c r="C29" s="8">
         <v>2</v>
       </c>
-      <c r="D29" s="18" t="s">
+      <c r="D29" s="3" t="s">
         <v>47</v>
       </c>
       <c r="E29" s="4" t="str">
@@ -3547,7 +3537,7 @@
       <c r="C30" s="10">
         <v>2</v>
       </c>
-      <c r="D30" s="21" t="s">
+      <c r="D30" s="5" t="s">
         <v>46</v>
       </c>
       <c r="E30" s="6" t="str">
@@ -3612,7 +3602,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>55</v>
       </c>
@@ -3639,7 +3629,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>55</v>
       </c>
@@ -3666,7 +3656,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>55</v>
       </c>
@@ -3693,7 +3683,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>55</v>
       </c>
@@ -3720,7 +3710,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>55</v>
       </c>
@@ -3738,7 +3728,7 @@
         <v>Prompt36</v>
       </c>
     </row>
-    <row r="38" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>55</v>
       </c>
@@ -3756,7 +3746,7 @@
         <v>Prompt37</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>55</v>
       </c>
@@ -3774,7 +3764,7 @@
         <v>Prompt38</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>55</v>
       </c>
@@ -3792,7 +3782,7 @@
         <v>Prompt39</v>
       </c>
     </row>
-    <row r="41" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>55</v>
       </c>
@@ -3810,932 +3800,959 @@
         <v>Prompt40</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="15" t="s">
+    <row r="42" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B42" t="s">
-        <v>97</v>
-      </c>
-      <c r="C42" s="16">
+      <c r="B42" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C42" s="8">
         <v>1</v>
       </c>
-      <c r="D42" s="15"/>
-      <c r="E42" s="17" t="str">
+      <c r="D42" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E42" s="4" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\1OSPF\router28.png","Prompt41")</f>
         <v>Prompt41</v>
       </c>
-      <c r="F42" s="15" t="s">
+      <c r="F42" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G42" s="15"/>
-      <c r="H42" s="15"/>
-      <c r="I42" s="15"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="15" t="s">
+    </row>
+    <row r="43" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B43" t="s">
-        <v>97</v>
-      </c>
-      <c r="C43" s="16">
+      <c r="B43" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C43" s="8">
         <v>1</v>
       </c>
-      <c r="D43" s="15"/>
-      <c r="E43" s="17" t="str">
+      <c r="D43" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E43" s="4" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\1OSPF\router29.png","Prompt42")</f>
         <v>Prompt42</v>
       </c>
-      <c r="F43" s="15" t="s">
+      <c r="F43" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="G43" s="15"/>
-      <c r="H43" s="15"/>
-      <c r="I43" s="15"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="15" t="s">
+    </row>
+    <row r="44" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B44" t="s">
-        <v>97</v>
-      </c>
-      <c r="C44" s="16">
+      <c r="B44" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C44" s="7">
         <v>1</v>
       </c>
-      <c r="D44" s="15"/>
-      <c r="E44" s="17" t="str">
+      <c r="D44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" s="2" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\1OSPF\router30.png","Prompt43")</f>
         <v>Prompt43</v>
       </c>
-      <c r="F44" s="15" t="s">
+      <c r="F44" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G44" s="15"/>
-      <c r="H44" s="15"/>
-      <c r="I44" s="15"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="15" t="s">
+    </row>
+    <row r="45" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B45" t="s">
-        <v>97</v>
-      </c>
-      <c r="C45" s="16">
+      <c r="B45" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C45" s="8">
         <v>1</v>
       </c>
-      <c r="D45" s="15"/>
-      <c r="E45" s="17" t="str">
+      <c r="D45" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E45" s="4" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\1OSPF\router31.png","Prompt44")</f>
         <v>Prompt44</v>
       </c>
-      <c r="F45" s="15" t="s">
+      <c r="F45" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="G45" s="15"/>
-      <c r="H45" s="15"/>
-      <c r="I45" s="15"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="15" t="s">
+    </row>
+    <row r="46" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B46" t="s">
-        <v>97</v>
-      </c>
-      <c r="C46" s="16">
+      <c r="B46" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C46" s="8">
         <v>1</v>
       </c>
-      <c r="D46" s="15"/>
-      <c r="E46" s="17" t="str">
+      <c r="D46" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E46" s="4" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\1OSPF\router32.png","Prompt45")</f>
         <v>Prompt45</v>
       </c>
-      <c r="F46" s="15" t="s">
+      <c r="F46" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="G46" s="15"/>
-      <c r="H46" s="15"/>
-      <c r="I46" s="15"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="15" t="s">
+    </row>
+    <row r="47" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B47" t="s">
-        <v>97</v>
-      </c>
-      <c r="C47" s="16">
+      <c r="B47" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C47" s="7">
         <v>2</v>
       </c>
-      <c r="D47" s="15"/>
-      <c r="E47" s="17" t="str">
+      <c r="D47" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" s="2" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\2OSPF\router40.png","Prompt46")</f>
         <v>Prompt46</v>
       </c>
-      <c r="F47" s="15" t="s">
+      <c r="F47" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G47" s="15" t="s">
+      <c r="G47" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H47" s="15"/>
-      <c r="I47" s="15"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="15" t="s">
+    </row>
+    <row r="48" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B48" t="s">
-        <v>97</v>
-      </c>
-      <c r="C48" s="16">
+      <c r="B48" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48" s="10">
         <v>2</v>
       </c>
-      <c r="D48" s="15"/>
-      <c r="E48" s="17" t="str">
+      <c r="D48" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E48" s="6" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\2OSPF\router41.png","Prompt47")</f>
         <v>Prompt47</v>
       </c>
-      <c r="F48" s="15" t="s">
+      <c r="F48" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="G48" s="15" t="s">
+      <c r="G48" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="H48" s="15"/>
-      <c r="I48" s="15"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="15" t="s">
+    </row>
+    <row r="49" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B49" t="s">
-        <v>97</v>
-      </c>
-      <c r="C49" s="16">
+      <c r="B49" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C49" s="7">
         <v>2</v>
       </c>
-      <c r="D49" s="15"/>
-      <c r="E49" s="17" t="str">
+      <c r="D49" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E49" s="2" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\2OSPF\router42.png","Prompt48")</f>
         <v>Prompt48</v>
       </c>
-      <c r="F49" s="15" t="s">
+      <c r="F49" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G49" s="15" t="s">
+      <c r="G49" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H49" s="15"/>
-      <c r="I49" s="15"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="15" t="s">
+    </row>
+    <row r="50" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B50" t="s">
-        <v>97</v>
-      </c>
-      <c r="C50" s="16">
+      <c r="B50" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C50" s="8">
         <v>2</v>
       </c>
-      <c r="D50" s="15"/>
-      <c r="E50" s="17" t="str">
+      <c r="D50" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E50" s="4" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\2OSPF\router43.png","Prompt49")</f>
         <v>Prompt49</v>
       </c>
-      <c r="F50" s="15" t="s">
+      <c r="F50" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G50" s="15" t="s">
+      <c r="G50" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="H50" s="15"/>
-      <c r="I50" s="15"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="15" t="s">
+    </row>
+    <row r="51" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B51" t="s">
-        <v>97</v>
-      </c>
-      <c r="C51" s="16">
+      <c r="B51" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C51" s="10">
         <v>2</v>
       </c>
-      <c r="D51" s="15"/>
-      <c r="E51" s="17" t="str">
+      <c r="D51" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E51" s="6" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMidt\2OSPF\router44.png","Prompt50")</f>
         <v>Prompt50</v>
       </c>
-      <c r="F51" s="15" t="s">
+      <c r="F51" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="G51" s="15" t="s">
+      <c r="G51" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="H51" s="15"/>
-      <c r="I51" s="15"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="15" t="s">
+    </row>
+    <row r="52" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B52" t="s">
-        <v>97</v>
-      </c>
-      <c r="C52" s="16">
+      <c r="B52" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C52" s="7">
         <v>3</v>
       </c>
-      <c r="D52" s="15"/>
-      <c r="E52" s="17" t="str">
+      <c r="D52" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" s="2" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\3OSPF\router46.png","Prompt51")</f>
         <v>Prompt51</v>
       </c>
-      <c r="F52" s="15" t="s">
+      <c r="F52" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G52" s="15" t="s">
+      <c r="G52" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H52" s="15" t="s">
+      <c r="H52" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I52" s="15"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="15" t="s">
+    </row>
+    <row r="53" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B53" t="s">
-        <v>97</v>
-      </c>
-      <c r="C53" s="16">
+      <c r="B53" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C53" s="8">
         <v>3</v>
       </c>
-      <c r="D53" s="15"/>
-      <c r="E53" s="17" t="str">
+      <c r="D53" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E53" s="4" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\3OSPF\router47.png","Prompt52")</f>
         <v>Prompt52</v>
       </c>
-      <c r="F53" s="15" t="s">
+      <c r="F53" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="G53" s="15" t="s">
+      <c r="G53" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="H53" s="15" t="s">
+      <c r="H53" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="I53" s="15"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="15" t="s">
+    </row>
+    <row r="54" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B54" t="s">
-        <v>97</v>
-      </c>
-      <c r="C54" s="16">
+      <c r="B54" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C54" s="10">
         <v>3</v>
       </c>
-      <c r="D54" s="15"/>
-      <c r="E54" s="17" t="str">
+      <c r="D54" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E54" s="6" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\3OSPF\router48.png","Prompt53")</f>
         <v>Prompt53</v>
       </c>
-      <c r="F54" s="15" t="s">
+      <c r="F54" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="G54" s="15" t="s">
+      <c r="G54" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="H54" s="15" t="s">
+      <c r="H54" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="I54" s="15"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="15" t="s">
+    </row>
+    <row r="55" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B55" t="s">
-        <v>97</v>
-      </c>
-      <c r="C55" s="16">
+      <c r="B55" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C55" s="10">
         <v>3</v>
       </c>
-      <c r="D55" s="15"/>
-      <c r="E55" s="17" t="str">
+      <c r="D55" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E55" s="6" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\3OSPF\router49.png","Prompt54")</f>
         <v>Prompt54</v>
       </c>
-      <c r="F55" s="15" t="s">
+      <c r="F55" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="G55" s="15" t="s">
+      <c r="G55" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="H55" s="15" t="s">
+      <c r="H55" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="I55" s="15"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="15" t="s">
+    </row>
+    <row r="56" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B56" t="s">
-        <v>97</v>
-      </c>
-      <c r="C56" s="16">
+      <c r="B56" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C56" s="10">
         <v>3</v>
       </c>
-      <c r="D56" s="15"/>
-      <c r="E56" s="17" t="str">
+      <c r="D56" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E56" s="6" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\3OSPF\router50.png","Prompt55")</f>
         <v>Prompt55</v>
       </c>
-      <c r="F56" s="15" t="s">
+      <c r="F56" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="G56" s="15" t="s">
+      <c r="G56" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="H56" s="15" t="s">
+      <c r="H56" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="I56" s="15"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="15" t="s">
+    </row>
+    <row r="57" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B57" t="s">
-        <v>97</v>
-      </c>
-      <c r="C57" s="16" t="s">
+      <c r="B57" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C57" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D57" s="15"/>
-      <c r="E57" s="17" t="str">
+      <c r="D57" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E57" s="2" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\OSPFMistype\router34.png","Prompt56")</f>
         <v>Prompt56</v>
       </c>
-      <c r="F57" s="15"/>
-      <c r="G57" s="15"/>
-      <c r="H57" s="15"/>
-      <c r="I57" s="15"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="15" t="s">
+    </row>
+    <row r="58" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B58" t="s">
-        <v>97</v>
-      </c>
-      <c r="C58" s="16" t="s">
+      <c r="B58" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C58" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D58" s="15"/>
-      <c r="E58" s="17" t="str">
+      <c r="D58" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E58" s="2" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\OSPFMistype\router35.png","Prompt57")</f>
         <v>Prompt57</v>
       </c>
-      <c r="F58" s="15"/>
-      <c r="G58" s="15"/>
-      <c r="H58" s="15"/>
-      <c r="I58" s="15"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="15" t="s">
+    </row>
+    <row r="59" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B59" t="s">
-        <v>97</v>
-      </c>
-      <c r="C59" s="16" t="s">
+      <c r="B59" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C59" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D59" s="15"/>
-      <c r="E59" s="17" t="str">
+      <c r="D59" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E59" s="2" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\OSPFMistype\router36.png","Prompt58")</f>
         <v>Prompt58</v>
       </c>
-      <c r="F59" s="15"/>
-      <c r="G59" s="15"/>
-      <c r="H59" s="15"/>
-      <c r="I59" s="15"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="15" t="s">
+    </row>
+    <row r="60" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B60" t="s">
-        <v>97</v>
-      </c>
-      <c r="C60" s="16" t="s">
+      <c r="B60" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C60" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D60" s="15"/>
-      <c r="E60" s="17" t="str">
+      <c r="D60" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E60" s="2" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\OSPFMistype\router37.png","Prompt59")</f>
         <v>Prompt59</v>
       </c>
-      <c r="F60" s="15"/>
-      <c r="G60" s="15"/>
-      <c r="H60" s="15"/>
-      <c r="I60" s="15"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="15" t="s">
+    </row>
+    <row r="61" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B61" t="s">
-        <v>97</v>
-      </c>
-      <c r="C61" s="16" t="s">
+      <c r="B61" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C61" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D61" s="15"/>
-      <c r="E61" s="17" t="str">
+      <c r="D61" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E61" s="4" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\OSPFMistype\router38.png","Prompt60")</f>
         <v>Prompt60</v>
       </c>
-      <c r="F61" s="15"/>
-      <c r="G61" s="15"/>
-      <c r="H61" s="15"/>
-      <c r="I61" s="15"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="15" t="s">
+    </row>
+    <row r="62" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B62" t="s">
-        <v>97</v>
-      </c>
-      <c r="C62" s="16">
+      <c r="B62" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C62" s="8">
         <v>1</v>
       </c>
-      <c r="D62" s="15"/>
-      <c r="E62" s="17" t="str">
+      <c r="D62" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E62" s="4" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\1RIP\router52.png","Prompt61")</f>
         <v>Prompt61</v>
       </c>
-      <c r="F62" s="15" t="s">
+      <c r="F62" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G62" s="15"/>
-      <c r="H62" s="15"/>
-      <c r="I62" s="15"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="15" t="s">
+    </row>
+    <row r="63" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B63" t="s">
-        <v>97</v>
-      </c>
-      <c r="C63" s="16">
+      <c r="B63" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C63" s="8">
         <v>1</v>
       </c>
-      <c r="D63" s="15"/>
-      <c r="E63" s="17" t="str">
+      <c r="D63" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E63" s="4" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\1RIP\router53.png","Prompt62")</f>
         <v>Prompt62</v>
       </c>
-      <c r="F63" s="15" t="s">
+      <c r="F63" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G63" s="15"/>
-      <c r="H63" s="15"/>
-      <c r="I63" s="15"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="15" t="s">
+    </row>
+    <row r="64" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B64" t="s">
-        <v>97</v>
-      </c>
-      <c r="C64" s="16">
+      <c r="B64" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C64" s="8">
         <v>1</v>
       </c>
-      <c r="D64" s="15"/>
-      <c r="E64" s="17" t="str">
+      <c r="D64" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E64" s="4" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\1RIP\router54.png","Prompt63")</f>
         <v>Prompt63</v>
       </c>
-      <c r="F64" s="15" t="s">
+      <c r="F64" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G64" s="15"/>
-      <c r="H64" s="15"/>
-      <c r="I64" s="15"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="15" t="s">
+    </row>
+    <row r="65" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B65" t="s">
-        <v>97</v>
-      </c>
-      <c r="C65" s="16">
+      <c r="B65" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C65" s="7">
         <v>1</v>
       </c>
-      <c r="D65" s="15"/>
-      <c r="E65" s="17" t="str">
+      <c r="D65" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E65" s="2" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\1RIP\router55.png","Prompt64")</f>
         <v>Prompt64</v>
       </c>
-      <c r="F65" s="15" t="s">
+      <c r="F65" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G65" s="15"/>
-      <c r="H65" s="15"/>
-      <c r="I65" s="15"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="15" t="s">
+    </row>
+    <row r="66" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B66" t="s">
-        <v>97</v>
-      </c>
-      <c r="C66" s="16">
+      <c r="B66" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C66" s="8">
         <v>1</v>
       </c>
-      <c r="D66" s="15"/>
-      <c r="E66" s="17" t="str">
+      <c r="D66" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E66" s="4" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\1RIP\router56.png","Prompt65")</f>
         <v>Prompt65</v>
       </c>
-      <c r="F66" s="15" t="s">
+      <c r="F66" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="G66" s="15"/>
-      <c r="H66" s="15"/>
-      <c r="I66" s="15"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="15" t="s">
+    </row>
+    <row r="67" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B67" t="s">
-        <v>97</v>
-      </c>
-      <c r="C67" s="16">
+      <c r="B67" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C67" s="8">
         <v>2</v>
       </c>
-      <c r="D67" s="15"/>
-      <c r="E67" s="17" t="str">
+      <c r="D67" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E67" s="4" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\1RIP\router58.png","Prompt66")</f>
         <v>Prompt66</v>
       </c>
-      <c r="F67" s="15" t="s">
+      <c r="F67" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G67" s="15" t="s">
+      <c r="G67" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H67" s="15"/>
-      <c r="I67" s="15"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="15" t="s">
+    </row>
+    <row r="68" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B68" t="s">
-        <v>97</v>
-      </c>
-      <c r="C68" s="16">
+      <c r="B68" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C68" s="7">
         <v>2</v>
       </c>
-      <c r="D68" s="15"/>
-      <c r="E68" s="17" t="str">
+      <c r="D68" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E68" s="2" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\1RIP\router59.png","Prompt67")</f>
         <v>Prompt67</v>
       </c>
-      <c r="F68" s="15" t="s">
+      <c r="F68" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G68" s="15" t="s">
+      <c r="G68" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H68" s="15"/>
-      <c r="I68" s="15"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="15" t="s">
+    </row>
+    <row r="69" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B69" t="s">
-        <v>97</v>
-      </c>
-      <c r="C69" s="16">
+      <c r="B69" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C69" s="8">
         <v>2</v>
       </c>
-      <c r="D69" s="15"/>
-      <c r="E69" s="17" t="str">
+      <c r="D69" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E69" s="4" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMidt\2RIP\router60.png","Prompt68")</f>
         <v>Prompt68</v>
       </c>
-      <c r="F69" s="15" t="s">
+      <c r="F69" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G69" s="15" t="s">
+      <c r="G69" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="H69" s="15"/>
-      <c r="I69" s="15"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="15" t="s">
+    </row>
+    <row r="70" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B70" t="s">
-        <v>97</v>
-      </c>
-      <c r="C70" s="16">
+      <c r="B70" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C70" s="10">
         <v>2</v>
       </c>
-      <c r="D70" s="15"/>
-      <c r="E70" s="17" t="str">
+      <c r="D70" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E70" s="6" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\2RIP\router61.png","Prompt69")</f>
         <v>Prompt69</v>
       </c>
-      <c r="F70" s="15" t="s">
+      <c r="F70" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="G70" s="15" t="s">
+      <c r="G70" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="H70" s="15"/>
-      <c r="I70" s="15"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="15" t="s">
+    </row>
+    <row r="71" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B71" t="s">
-        <v>97</v>
-      </c>
-      <c r="C71" s="16">
+      <c r="B71" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C71" s="10">
         <v>2</v>
       </c>
-      <c r="D71" s="15"/>
-      <c r="E71" s="17" t="str">
+      <c r="D71" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E71" s="6" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\2RIP\router62.png","Prompt70")</f>
         <v>Prompt70</v>
       </c>
-      <c r="F71" s="15" t="s">
+      <c r="F71" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="G71" s="15" t="s">
+      <c r="G71" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H71" s="15"/>
-      <c r="I71" s="15"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="15" t="s">
+    </row>
+    <row r="72" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B72" t="s">
-        <v>97</v>
-      </c>
-      <c r="C72" s="16">
+      <c r="B72" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C72" s="8">
         <v>3</v>
       </c>
-      <c r="D72" s="15"/>
-      <c r="E72" s="17" t="str">
+      <c r="D72" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E72" s="4" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\3RIP\router62.png","Prompt71")</f>
         <v>Prompt71</v>
       </c>
-      <c r="F72" s="15" t="s">
+      <c r="F72" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G72" s="15" t="s">
+      <c r="G72" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H72" s="15" t="s">
+      <c r="H72" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="I72" s="15"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="15" t="s">
+    </row>
+    <row r="73" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B73" t="s">
-        <v>97</v>
-      </c>
-      <c r="C73" s="16">
+      <c r="B73" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C73" s="8">
         <v>3</v>
       </c>
-      <c r="D73" s="15"/>
-      <c r="E73" s="17" t="str">
+      <c r="D73" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E73" s="4" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\3RIP\router63.png","Prompt72")</f>
         <v>Prompt72</v>
       </c>
-      <c r="F73" s="15" t="s">
+      <c r="F73" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="G73" s="15" t="s">
+      <c r="G73" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="H73" s="15" t="s">
+      <c r="H73" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="I73" s="15"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="15" t="s">
+    </row>
+    <row r="74" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B74" t="s">
-        <v>97</v>
-      </c>
-      <c r="C74" s="16">
+      <c r="B74" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C74" s="8">
         <v>3</v>
       </c>
-      <c r="D74" s="15"/>
-      <c r="E74" s="17" t="str">
+      <c r="D74" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E74" s="4" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\3RIP\router64.png","Prompt73")</f>
         <v>Prompt73</v>
       </c>
-      <c r="F74" s="15" t="s">
+      <c r="F74" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="G74" s="15" t="s">
+      <c r="G74" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="H74" s="15" t="s">
+      <c r="H74" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="I74" s="15"/>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="15" t="s">
+    </row>
+    <row r="75" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B75" t="s">
-        <v>97</v>
-      </c>
-      <c r="C75" s="16">
+      <c r="B75" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C75" s="8">
         <v>3</v>
       </c>
-      <c r="D75" s="15"/>
-      <c r="E75" s="17" t="str">
+      <c r="D75" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E75" s="4" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\3RIP\router65.png","Prompt74")</f>
         <v>Prompt74</v>
       </c>
-      <c r="F75" s="15" t="s">
+      <c r="F75" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G75" s="15" t="s">
+      <c r="G75" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="H75" s="15" t="s">
+      <c r="H75" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="I75" s="15"/>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="15" t="s">
+    </row>
+    <row r="76" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B76" t="s">
-        <v>97</v>
-      </c>
-      <c r="C76" s="16">
+      <c r="B76" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C76" s="8">
         <v>3</v>
       </c>
-      <c r="D76" s="15"/>
-      <c r="E76" s="17" t="str">
+      <c r="D76" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E76" s="4" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\3RIP\router66.png","Prompt75")</f>
         <v>Prompt75</v>
       </c>
-      <c r="F76" s="15" t="s">
+      <c r="F76" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G76" s="15" t="s">
+      <c r="G76" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="H76" s="15" t="s">
+      <c r="H76" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="I76" s="15"/>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="15" t="s">
+    </row>
+    <row r="77" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B77" t="s">
-        <v>97</v>
-      </c>
-      <c r="C77" s="16" t="s">
+      <c r="B77" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C77" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D77" s="15"/>
-      <c r="E77" s="17" t="str">
+      <c r="D77" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E77" s="2" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\RIPMistype\router52.png","Prompt76")</f>
         <v>Prompt76</v>
       </c>
-      <c r="F77" s="15"/>
-      <c r="G77" s="15"/>
-      <c r="H77" s="15"/>
-      <c r="I77" s="15"/>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="15" t="s">
+    </row>
+    <row r="78" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B78" t="s">
-        <v>97</v>
-      </c>
-      <c r="C78" s="16" t="s">
+      <c r="B78" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C78" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D78" s="15"/>
-      <c r="E78" s="17" t="str">
+      <c r="D78" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E78" s="2" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\RIPMistype\router53.png","Prompt77")</f>
         <v>Prompt77</v>
       </c>
-      <c r="F78" s="15"/>
-      <c r="G78" s="15"/>
-      <c r="H78" s="15"/>
-      <c r="I78" s="15"/>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="15" t="s">
+    </row>
+    <row r="79" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B79" t="s">
-        <v>97</v>
-      </c>
-      <c r="C79" s="16" t="s">
+      <c r="B79" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C79" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D79" s="15"/>
-      <c r="E79" s="17" t="str">
+      <c r="D79" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E79" s="2" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\RIPMistype\router54.png","Prompt78")</f>
         <v>Prompt78</v>
       </c>
-      <c r="F79" s="15"/>
-      <c r="G79" s="15"/>
-      <c r="H79" s="15"/>
-      <c r="I79" s="15"/>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="15" t="s">
+    </row>
+    <row r="80" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B80" t="s">
-        <v>97</v>
-      </c>
-      <c r="C80" s="16" t="s">
+      <c r="B80" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C80" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D80" s="15"/>
-      <c r="E80" s="17" t="str">
+      <c r="D80" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E80" s="2" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\RIPMistype\router55.png","Prompt79")</f>
         <v>Prompt79</v>
       </c>
-      <c r="F80" s="15"/>
-      <c r="G80" s="15"/>
-      <c r="H80" s="15"/>
-      <c r="I80" s="15"/>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" s="15" t="s">
+    </row>
+    <row r="81" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B81" t="s">
-        <v>97</v>
-      </c>
-      <c r="C81" s="16" t="s">
+      <c r="B81" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C81" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D81" s="15"/>
-      <c r="E81" s="17" t="str">
+      <c r="D81" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E81" s="4" t="str">
         <f>HYPERLINK("Z:\Thesis\PromptMid\RIPMistype\router56.png","Prompt80")</f>
         <v>Prompt80</v>
       </c>
-      <c r="F81" s="15"/>
-      <c r="G81" s="15"/>
-      <c r="H81" s="15"/>
-      <c r="I81" s="15"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C83" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D83" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="E83" s="14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B84" s="11">
+        <v>120</v>
+      </c>
+      <c r="C84" s="11">
+        <v>39</v>
+      </c>
+      <c r="D84" s="11">
+        <v>81</v>
+      </c>
+      <c r="E84" s="13">
+        <f>C84/B84</f>
+        <v>0.32500000000000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B85" s="11">
+        <v>20</v>
+      </c>
+      <c r="C85" s="11">
+        <v>17</v>
+      </c>
+      <c r="D85" s="11">
+        <v>3</v>
+      </c>
+      <c r="E85" s="13">
+        <f>C85/B85</f>
+        <v>0.85</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C81" xr:uid="{1C1A52BA-925C-4174-AD08-B6CE84EE4C4B}">
       <formula1>"1, 2, 3, Mistype"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A81" xr:uid="{FB8643A0-7E18-40C0-92D4-0D07C8EB94FB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A81 A83" xr:uid="{FB8643A0-7E18-40C0-92D4-0D07C8EB94FB}">
       <formula1>"AAA, EIGRP, VLAN, OSPF, RIP"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D8 D10:D81" xr:uid="{746F0A84-D670-407A-B7E1-03C7A97A34D2}">
@@ -4780,7 +4797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9844366C-8411-40C3-A46E-192183A9621E}">
   <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Methodology Draft + PP Score Update
Somewhat finished the Methodology Draft 1 and added individual PP scores for each protocol in the Results excel sheet
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Repo\Dissertation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C49FC1-7F9E-421C-B959-D3FFEA5FB0DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC3EEA4-96EA-4AC5-B711-DCEF35B8848F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{6E62CC2F-5E46-4B0F-9F3F-D109107C993D}"/>
+    <workbookView xWindow="-21675" yWindow="2550" windowWidth="21600" windowHeight="11835" activeTab="2" xr2:uid="{6E62CC2F-5E46-4B0F-9F3F-D109107C993D}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1277" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="103">
   <si>
     <t>Section</t>
   </si>
@@ -378,6 +378,21 @@
   <si>
     <t>You are a network security analyst reviewing a router configuration for deployment in a mid-sized corporate network. Task: According to CIS Benchmarks is this configuration secure? Please identify any security issues, misconfigurations, typos, or best practice violations. If the configuration is secure, state: "Yes, this configuration appears secure." Otherwise, explain the issues briefly.</t>
   </si>
+  <si>
+    <t>TotalErrors</t>
+  </si>
+  <si>
+    <t>AAA Errors</t>
+  </si>
+  <si>
+    <t>EIGRP Errors</t>
+  </si>
+  <si>
+    <t>OSPF Errors</t>
+  </si>
+  <si>
+    <t>RIP Errors</t>
+  </si>
 </sst>
 </file>
 
@@ -423,7 +438,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -460,6 +475,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF222909"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -475,7 +502,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
@@ -504,6 +531,14 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -513,7 +548,74 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
     <mruColors>
+      <color rgb="FF222909"/>
       <color rgb="FFDC2860"/>
     </mruColors>
   </colors>
@@ -533,10 +635,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="C0C0C0"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="191919"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -845,14 +947,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E456A3C5-04F2-4269-B1CC-66B09066F0AA}">
-  <dimension ref="A1:I86"/>
+  <dimension ref="A1:I91"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83:E85"/>
+    <sheetView topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E91" sqref="A85:E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
     <col min="2" max="2" width="56" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" style="9" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" customWidth="1"/>
@@ -2722,68 +2825,134 @@
         <v>Prompt80</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C83" s="12" t="s">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C85" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="D83" s="12" t="s">
+      <c r="D85" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="E83" s="14" t="s">
+      <c r="E85" s="14" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B84" s="11">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B86" s="18">
+        <v>30</v>
+      </c>
+      <c r="C86" s="18">
+        <v>12</v>
+      </c>
+      <c r="D86" s="18">
+        <v>18</v>
+      </c>
+      <c r="E86" s="19">
+        <f>C86/B86</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B87" s="18">
+        <v>30</v>
+      </c>
+      <c r="C87" s="18">
+        <v>1</v>
+      </c>
+      <c r="D87" s="18">
+        <v>29</v>
+      </c>
+      <c r="E87" s="19">
+        <f>C87/B87</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B88" s="18">
+        <v>30</v>
+      </c>
+      <c r="C88" s="18">
+        <v>17</v>
+      </c>
+      <c r="D88" s="18">
+        <v>13</v>
+      </c>
+      <c r="E88" s="19">
+        <f>C88/B88</f>
+        <v>0.56666666666666665</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B89" s="18">
+        <v>30</v>
+      </c>
+      <c r="C89" s="18">
+        <v>3</v>
+      </c>
+      <c r="D89" s="18">
+        <v>27</v>
+      </c>
+      <c r="E89" s="19">
+        <f>C89/B89</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B90" s="16">
         <v>120</v>
       </c>
-      <c r="C84" s="11">
+      <c r="C90" s="16">
         <v>34</v>
       </c>
-      <c r="D84" s="11">
+      <c r="D90" s="16">
         <v>86</v>
       </c>
-      <c r="E84" s="13">
-        <f>C84/B84</f>
+      <c r="E90" s="17">
+        <f>C90/B90</f>
         <v>0.28333333333333333</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="11" t="s">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="B85" s="11">
+      <c r="B91" s="16">
         <v>20</v>
       </c>
-      <c r="C85" s="11">
+      <c r="C91" s="16">
         <v>15</v>
       </c>
-      <c r="D85" s="11">
+      <c r="D91" s="16">
         <v>5</v>
       </c>
-      <c r="E85" s="13">
-        <f>C85/B85</f>
+      <c r="E91" s="17">
+        <f>C91/B91</f>
         <v>0.75</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="11"/>
-      <c r="B86" s="11"/>
-      <c r="C86" s="11"/>
-      <c r="D86" s="11"/>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A83 A86:A1048576" xr:uid="{960B71D9-6483-4016-80B8-B49529829EEE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A83 A92:A1048576" xr:uid="{960B71D9-6483-4016-80B8-B49529829EEE}">
       <formula1>"AAA, EIGRP, VLAN, OSPF, RIP"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C86:C1048576 C1:C82" xr:uid="{C6ABE5CC-E54D-4270-B42B-0010339E196E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C82 C92:C1048576" xr:uid="{C6ABE5CC-E54D-4270-B42B-0010339E196E}">
       <formula1>"1, 2, 3, Mistype"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D86:D1048576 D1:D82" xr:uid="{3EFC7604-AA39-474F-B024-363A9AA03EDF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D82 D92:D1048576" xr:uid="{3EFC7604-AA39-474F-B024-363A9AA03EDF}">
       <formula1>"Yes, No, 1 Error, 2 Error"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2824,14 +2993,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F11B0BFB-3F43-4298-9582-F5223F20D3AC}">
-  <dimension ref="A1:I85"/>
+  <dimension ref="A1:I89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D88" sqref="D88"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83:E89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="44" customWidth="1"/>
     <col min="3" max="3" width="19.140625" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
@@ -4712,38 +4882,110 @@
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B84" s="11">
+      <c r="A84" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B84" s="18">
+        <v>30</v>
+      </c>
+      <c r="C84" s="18">
+        <v>11</v>
+      </c>
+      <c r="D84" s="18">
+        <v>19</v>
+      </c>
+      <c r="E84" s="19">
+        <f>C84/B84</f>
+        <v>0.36666666666666664</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B85" s="18">
+        <v>30</v>
+      </c>
+      <c r="C85" s="18">
+        <v>10</v>
+      </c>
+      <c r="D85" s="18">
+        <v>20</v>
+      </c>
+      <c r="E85" s="19">
+        <f>C85/B85</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B86" s="18">
+        <v>30</v>
+      </c>
+      <c r="C86" s="18">
+        <v>15</v>
+      </c>
+      <c r="D86" s="18">
+        <v>15</v>
+      </c>
+      <c r="E86" s="19">
+        <f>C86/B86</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B87" s="18">
+        <v>30</v>
+      </c>
+      <c r="C87" s="18">
+        <v>5</v>
+      </c>
+      <c r="D87" s="18">
+        <v>25</v>
+      </c>
+      <c r="E87" s="19">
+        <f>C87/B87</f>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B88" s="16">
         <v>120</v>
       </c>
-      <c r="C84" s="11">
+      <c r="C88" s="16">
         <v>39</v>
       </c>
-      <c r="D84" s="11">
+      <c r="D88" s="16">
         <v>81</v>
       </c>
-      <c r="E84" s="13">
-        <f>C84/B84</f>
+      <c r="E88" s="17">
+        <f>C88/B88</f>
         <v>0.32500000000000001</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="11" t="s">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="B85" s="11">
+      <c r="B89" s="16">
         <v>20</v>
       </c>
-      <c r="C85" s="11">
+      <c r="C89" s="16">
         <v>17</v>
       </c>
-      <c r="D85" s="11">
+      <c r="D89" s="16">
         <v>3</v>
       </c>
-      <c r="E85" s="13">
-        <f>C85/B85</f>
+      <c r="E89" s="17">
+        <f>C89/B89</f>
         <v>0.85</v>
       </c>
     </row>
@@ -4752,7 +4994,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C81" xr:uid="{1C1A52BA-925C-4174-AD08-B6CE84EE4C4B}">
       <formula1>"1, 2, 3, Mistype"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A81 A83" xr:uid="{FB8643A0-7E18-40C0-92D4-0D07C8EB94FB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A81" xr:uid="{FB8643A0-7E18-40C0-92D4-0D07C8EB94FB}">
       <formula1>"AAA, EIGRP, VLAN, OSPF, RIP"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D8 D10:D81" xr:uid="{746F0A84-D670-407A-B7E1-03C7A97A34D2}">
@@ -4795,10 +5037,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9844366C-8411-40C3-A46E-192183A9621E}">
-  <dimension ref="A1:I85"/>
+  <dimension ref="A1:I93"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="F90" sqref="F90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6719,15 +6961,134 @@
         <v>0.85</v>
       </c>
     </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C87" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D87" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="E87" s="14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B88" s="18">
+        <v>30</v>
+      </c>
+      <c r="C88" s="18">
+        <v>15</v>
+      </c>
+      <c r="D88" s="18">
+        <v>15</v>
+      </c>
+      <c r="E88" s="19">
+        <f>C88/B88</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B89" s="18">
+        <v>30</v>
+      </c>
+      <c r="C89" s="18">
+        <v>22</v>
+      </c>
+      <c r="D89" s="18">
+        <v>8</v>
+      </c>
+      <c r="E89" s="19">
+        <f>C89/B89</f>
+        <v>0.73333333333333328</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B90" s="18">
+        <v>30</v>
+      </c>
+      <c r="C90" s="18">
+        <v>23</v>
+      </c>
+      <c r="D90" s="18">
+        <v>7</v>
+      </c>
+      <c r="E90" s="19">
+        <f>C90/B90</f>
+        <v>0.76666666666666672</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B91" s="18">
+        <v>30</v>
+      </c>
+      <c r="C91" s="18">
+        <v>13</v>
+      </c>
+      <c r="D91" s="18">
+        <v>17</v>
+      </c>
+      <c r="E91" s="19">
+        <f>C91/B91</f>
+        <v>0.43333333333333335</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B92" s="16">
+        <v>120</v>
+      </c>
+      <c r="C92" s="16">
+        <v>73</v>
+      </c>
+      <c r="D92" s="16">
+        <v>47</v>
+      </c>
+      <c r="E92" s="17">
+        <f>C92/B92</f>
+        <v>0.60833333333333328</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B93" s="16">
+        <v>20</v>
+      </c>
+      <c r="C93" s="16">
+        <v>17</v>
+      </c>
+      <c r="D93" s="16">
+        <v>3</v>
+      </c>
+      <c r="E93" s="17">
+        <f>C93/B93</f>
+        <v>0.85</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D82 D86:D1048576" xr:uid="{736FCE3B-EAAD-48DE-8F70-E31CEAA49A0A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D82 D86 D94:D1048576" xr:uid="{736FCE3B-EAAD-48DE-8F70-E31CEAA49A0A}">
       <formula1>"Yes, No, 1 Error, 2 Error"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C82 C86:C1048576" xr:uid="{48F8CC9F-812E-49E3-A031-3AB70110A9DA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C82 C86 C94:C1048576" xr:uid="{48F8CC9F-812E-49E3-A031-3AB70110A9DA}">
       <formula1>"1, 2, 3, Mistype"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A86:A1048576 A1:A82" xr:uid="{8F9D317C-F984-4E77-BD5B-1B6802F8C843}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A82 A86 A94:A1048576" xr:uid="{8F9D317C-F984-4E77-BD5B-1B6802F8C843}">
       <formula1>"AAA, EIGRP, VLAN, OSPF, RIP"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>